<commit_message>
added graphing script for mach data
</commit_message>
<xml_diff>
--- a/AGCO/AGCO.xlsx
+++ b/AGCO/AGCO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32906c935fa0eb4f/models/AGCO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1242" documentId="11_F25DC773A252ABDACC104889191A52245ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DAFEE0B-64AF-45CB-85AF-4747104B7372}"/>
+  <xr:revisionPtr revIDLastSave="1243" documentId="11_F25DC773A252ABDACC104889191A52245ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A3E3FBA-CEEC-4342-B23C-87B6541815F1}"/>
   <bookViews>
-    <workbookView xWindow="11500" yWindow="5120" windowWidth="18000" windowHeight="12750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10530" yWindow="3610" windowWidth="12330" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1207,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7AD8E5B-022C-42CE-B268-F739C26FDB37}">
   <dimension ref="A1:M131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1927,6 +1927,9 @@
       </c>
     </row>
     <row r="30" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
@@ -1943,8 +1946,8 @@
       <c r="M30" s="15"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
-        <v>29</v>
+      <c r="A31" t="s">
+        <v>30</v>
       </c>
       <c r="B31" s="13">
         <v>3333.5</v>
@@ -1986,7 +1989,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="13">
         <v>2478.6</v>
@@ -2027,8 +2030,8 @@
       </c>
     </row>
     <row r="33" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>31</v>
+      <c r="A33" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B33" s="15">
         <f>B31-B32</f>
@@ -2079,8 +2082,8 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
-        <v>32</v>
+      <c r="A34" t="s">
+        <v>33</v>
       </c>
       <c r="B34" s="13">
         <v>331.8</v>
@@ -2122,7 +2125,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="B35" s="13">
         <v>119.6</v>
@@ -2164,7 +2167,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="B36" s="13">
         <v>14.8</v>
@@ -2206,7 +2209,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>116</v>
       </c>
       <c r="B37" s="13">
         <v>0</v>
@@ -2248,7 +2251,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>35</v>
       </c>
       <c r="B38" s="13">
         <v>1.4</v>
@@ -2290,7 +2293,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>117</v>
       </c>
       <c r="B39" s="13">
         <v>0</v>
@@ -2331,8 +2334,8 @@
       </c>
     </row>
     <row r="40" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>117</v>
+      <c r="A40" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B40" s="15">
         <f>SUM(B34:B38)+B32</f>
@@ -2384,7 +2387,7 @@
     </row>
     <row r="41" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B41" s="15">
         <f>B31-B40</f>
@@ -2435,8 +2438,8 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>36</v>
+      <c r="A42" t="s">
+        <v>37</v>
       </c>
       <c r="B42" s="13">
         <v>0.5</v>
@@ -2478,7 +2481,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B43" s="13">
         <v>50.4</v>
@@ -2519,8 +2522,8 @@
       </c>
     </row>
     <row r="44" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>38</v>
+      <c r="A44" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B44" s="15">
         <f>B41-B43-B42</f>
@@ -2571,8 +2574,8 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>39</v>
+      <c r="A45" t="s">
+        <v>45</v>
       </c>
       <c r="B45" s="13">
         <v>120.2</v>
@@ -2614,7 +2617,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B46" s="13">
         <v>16.399999999999999</v>
@@ -2656,7 +2659,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B47" s="13">
         <v>0</v>
@@ -2697,8 +2700,8 @@
       </c>
     </row>
     <row r="48" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>46</v>
+      <c r="A48" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B48" s="15">
         <f t="shared" ref="B48:F48" si="35">B44-B45+B46+B47</f>
@@ -2749,9 +2752,6 @@
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
@@ -2768,7 +2768,9 @@
       <c r="M49" s="13"/>
     </row>
     <row r="50" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50"/>
+      <c r="A50" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="B50" s="15">
         <f>B48/B54</f>
         <v>3.1179624664879388</v>
@@ -2819,7 +2821,7 @@
     </row>
     <row r="51" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B51" s="15">
         <f>B48/B55</f>
@@ -2870,8 +2872,8 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
-        <v>48</v>
+      <c r="A52" t="s">
+        <v>51</v>
       </c>
       <c r="B52" s="13">
         <v>0.24</v>
@@ -2912,14 +2914,14 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>51</v>
-      </c>
       <c r="J53" s="18" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>49</v>
+      </c>
       <c r="B54">
         <v>74.599999999999994</v>
       </c>
@@ -2956,7 +2958,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B55">
         <v>74.7</v>
@@ -2993,15 +2995,11 @@
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>50</v>
-      </c>
       <c r="J56" s="18" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57"/>
       <c r="B57" s="1" t="str">
         <f>B29</f>
         <v>Q123</v>
@@ -3051,12 +3049,14 @@
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A58" s="1"/>
       <c r="J58" s="18" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>52</v>
+      </c>
       <c r="B59" s="2">
         <v>232.6</v>
       </c>
@@ -3101,7 +3101,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B60" s="2">
         <f>53.6+14.8</f>
@@ -3149,7 +3149,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B61" s="2">
         <v>14</v>
@@ -3195,7 +3195,7 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="B62" s="2">
         <v>0</v>
@@ -3239,7 +3239,7 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B63" s="2">
         <v>0</v>
@@ -3283,7 +3283,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>121</v>
+        <v>55</v>
       </c>
       <c r="B64" s="2">
         <v>-16.399999999999999</v>
@@ -3329,7 +3329,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B65" s="2">
         <v>-3.9</v>
@@ -3375,7 +3375,7 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B66" s="2">
         <v>2.4</v>
@@ -3421,7 +3421,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B67" s="2">
         <v>-298.10000000000002</v>
@@ -3467,7 +3467,7 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B68" s="2">
         <v>-402.6</v>
@@ -3513,7 +3513,7 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B69" s="2">
         <v>-69.900000000000006</v>
@@ -3559,7 +3559,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B70" s="2">
         <v>39.200000000000003</v>
@@ -3605,7 +3605,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B71" s="2">
         <v>-155.9</v>
@@ -3651,7 +3651,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B72" s="2">
         <v>33.1</v>
@@ -3696,8 +3696,8 @@
       </c>
     </row>
     <row r="73" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>63</v>
+      <c r="A73" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="B73" s="3">
         <f>SUM(B59:B72)</f>
@@ -3748,9 +3748,6 @@
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A74" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="J74" s="18" t="s">
         <v>139</v>
       </c>

</xml_diff>